<commit_message>
update bets to hit to include current odds
</commit_message>
<xml_diff>
--- a/betting_lines_open_2025.xlsx
+++ b/betting_lines_open_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\Football-DNA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C21FCE4-D183-4A39-9AAD-E3019729F181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{197AF8FE-7502-4418-9F42-5CBD49763561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="1" xr2:uid="{38E66C5D-58C4-4402-8F4D-2FF7B602BD04}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="168">
   <si>
     <t>game</t>
   </si>
@@ -499,6 +499,48 @@
   </si>
   <si>
     <t>PHI_GB</t>
+  </si>
+  <si>
+    <t>NYJ_NE</t>
+  </si>
+  <si>
+    <t>WAS_MIA</t>
+  </si>
+  <si>
+    <t>GB_NYG</t>
+  </si>
+  <si>
+    <t>TB_BUF</t>
+  </si>
+  <si>
+    <t>HOU_TEN</t>
+  </si>
+  <si>
+    <t>CHI_MIN</t>
+  </si>
+  <si>
+    <t>CAR_ATL</t>
+  </si>
+  <si>
+    <t>LAC_JAX</t>
+  </si>
+  <si>
+    <t>SEA_LA</t>
+  </si>
+  <si>
+    <t>SF_ARI</t>
+  </si>
+  <si>
+    <t>BAL_CLE</t>
+  </si>
+  <si>
+    <t>KC_DEN</t>
+  </si>
+  <si>
+    <t>DET_PHI</t>
+  </si>
+  <si>
+    <t>DAL_LV</t>
   </si>
 </sst>
 </file>
@@ -1061,10 +1103,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FD36202-D83D-42C3-9E22-D680F63FC59E}">
-  <dimension ref="A1:D134"/>
+  <dimension ref="A1:D149"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D134" sqref="D134"/>
+    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
+      <selection activeCell="E138" sqref="E138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2945,6 +2987,216 @@
         <v>-1.5</v>
       </c>
     </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A135">
+        <v>11</v>
+      </c>
+      <c r="B135" t="s">
+        <v>154</v>
+      </c>
+      <c r="C135">
+        <v>42.5</v>
+      </c>
+      <c r="D135">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A136">
+        <v>11</v>
+      </c>
+      <c r="B136" t="s">
+        <v>155</v>
+      </c>
+      <c r="C136">
+        <v>48.5</v>
+      </c>
+      <c r="D136">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A137">
+        <v>11</v>
+      </c>
+      <c r="B137" t="s">
+        <v>156</v>
+      </c>
+      <c r="C137">
+        <v>43.5</v>
+      </c>
+      <c r="D137">
+        <v>-4.5</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A138">
+        <v>11</v>
+      </c>
+      <c r="B138" t="s">
+        <v>157</v>
+      </c>
+      <c r="C138">
+        <v>49.5</v>
+      </c>
+      <c r="D138">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A139">
+        <v>11</v>
+      </c>
+      <c r="B139" t="s">
+        <v>98</v>
+      </c>
+      <c r="C139">
+        <v>48.5</v>
+      </c>
+      <c r="D139">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A140">
+        <v>11</v>
+      </c>
+      <c r="B140" t="s">
+        <v>158</v>
+      </c>
+      <c r="C140">
+        <v>43.5</v>
+      </c>
+      <c r="D140">
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A141">
+        <v>11</v>
+      </c>
+      <c r="B141" t="s">
+        <v>159</v>
+      </c>
+      <c r="C141">
+        <v>45.5</v>
+      </c>
+      <c r="D141">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A142">
+        <v>11</v>
+      </c>
+      <c r="B142" t="s">
+        <v>160</v>
+      </c>
+      <c r="C142">
+        <v>45.5</v>
+      </c>
+      <c r="D142">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A143">
+        <v>11</v>
+      </c>
+      <c r="B143" t="s">
+        <v>161</v>
+      </c>
+      <c r="C143">
+        <v>46.5</v>
+      </c>
+      <c r="D143">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A144">
+        <v>11</v>
+      </c>
+      <c r="B144" t="s">
+        <v>162</v>
+      </c>
+      <c r="C144">
+        <v>45.5</v>
+      </c>
+      <c r="D144">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A145">
+        <v>11</v>
+      </c>
+      <c r="B145" t="s">
+        <v>163</v>
+      </c>
+      <c r="C145">
+        <v>47.5</v>
+      </c>
+      <c r="D145">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A146">
+        <v>11</v>
+      </c>
+      <c r="B146" t="s">
+        <v>164</v>
+      </c>
+      <c r="C146">
+        <v>44.5</v>
+      </c>
+      <c r="D146">
+        <v>-8.5</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A147">
+        <v>11</v>
+      </c>
+      <c r="B147" t="s">
+        <v>165</v>
+      </c>
+      <c r="C147">
+        <v>45.5</v>
+      </c>
+      <c r="D147">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A148">
+        <v>11</v>
+      </c>
+      <c r="B148" t="s">
+        <v>166</v>
+      </c>
+      <c r="C148">
+        <v>47.5</v>
+      </c>
+      <c r="D148">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A149">
+        <v>11</v>
+      </c>
+      <c r="B149" t="s">
+        <v>167</v>
+      </c>
+      <c r="C149">
+        <v>45.5</v>
+      </c>
+      <c r="D149">
+        <v>-1.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated for week 12
</commit_message>
<xml_diff>
--- a/betting_lines_open_2025.xlsx
+++ b/betting_lines_open_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\Football-DNA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{197AF8FE-7502-4418-9F42-5CBD49763561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E769E31F-6F2E-44B4-9428-CD67B7365576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="1" xr2:uid="{38E66C5D-58C4-4402-8F4D-2FF7B602BD04}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="182">
   <si>
     <t>game</t>
   </si>
@@ -541,6 +541,48 @@
   </si>
   <si>
     <t>DAL_LV</t>
+  </si>
+  <si>
+    <t>BUF_HOU</t>
+  </si>
+  <si>
+    <t>PIT_CHI</t>
+  </si>
+  <si>
+    <t>NYJ_BAL</t>
+  </si>
+  <si>
+    <t>NYG_DET</t>
+  </si>
+  <si>
+    <t>NE_CIN</t>
+  </si>
+  <si>
+    <t>SEA_TEN</t>
+  </si>
+  <si>
+    <t>MIN_GB</t>
+  </si>
+  <si>
+    <t>IND_KC</t>
+  </si>
+  <si>
+    <t>JAX_ARI</t>
+  </si>
+  <si>
+    <t>CLE_LV</t>
+  </si>
+  <si>
+    <t>ATL_NO</t>
+  </si>
+  <si>
+    <t>PHI_DAL</t>
+  </si>
+  <si>
+    <t>TB_LA</t>
+  </si>
+  <si>
+    <t>CAR_SF</t>
   </si>
 </sst>
 </file>
@@ -1103,10 +1145,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FD36202-D83D-42C3-9E22-D680F63FC59E}">
-  <dimension ref="A1:D149"/>
+  <dimension ref="A1:D163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
-      <selection activeCell="E138" sqref="E138"/>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="C149" sqref="C149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3197,6 +3239,202 @@
         <v>-1.5</v>
       </c>
     </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A150">
+        <v>12</v>
+      </c>
+      <c r="B150" t="s">
+        <v>168</v>
+      </c>
+      <c r="C150">
+        <v>46.5</v>
+      </c>
+      <c r="D150">
+        <v>-3.5</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A151">
+        <v>12</v>
+      </c>
+      <c r="B151" t="s">
+        <v>169</v>
+      </c>
+      <c r="C151">
+        <v>44.5</v>
+      </c>
+      <c r="D151">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A152">
+        <v>12</v>
+      </c>
+      <c r="B152" t="s">
+        <v>170</v>
+      </c>
+      <c r="C152">
+        <v>44.5</v>
+      </c>
+      <c r="D152">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A153">
+        <v>12</v>
+      </c>
+      <c r="B153" t="s">
+        <v>171</v>
+      </c>
+      <c r="C153">
+        <v>45.5</v>
+      </c>
+      <c r="D153">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A154">
+        <v>12</v>
+      </c>
+      <c r="B154" t="s">
+        <v>172</v>
+      </c>
+      <c r="C154">
+        <v>47.5</v>
+      </c>
+      <c r="D154">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A155">
+        <v>12</v>
+      </c>
+      <c r="B155" t="s">
+        <v>173</v>
+      </c>
+      <c r="C155">
+        <v>44.5</v>
+      </c>
+      <c r="D155">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A156">
+        <v>12</v>
+      </c>
+      <c r="B156" t="s">
+        <v>174</v>
+      </c>
+      <c r="C156">
+        <v>45.5</v>
+      </c>
+      <c r="D156">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A157">
+        <v>12</v>
+      </c>
+      <c r="B157" t="s">
+        <v>175</v>
+      </c>
+      <c r="C157">
+        <v>45.5</v>
+      </c>
+      <c r="D157">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A158">
+        <v>12</v>
+      </c>
+      <c r="B158" t="s">
+        <v>176</v>
+      </c>
+      <c r="C158">
+        <v>47.5</v>
+      </c>
+      <c r="D158">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A159">
+        <v>12</v>
+      </c>
+      <c r="B159" t="s">
+        <v>177</v>
+      </c>
+      <c r="C159">
+        <v>41.5</v>
+      </c>
+      <c r="D159">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A160">
+        <v>12</v>
+      </c>
+      <c r="B160" t="s">
+        <v>178</v>
+      </c>
+      <c r="C160">
+        <v>43.5</v>
+      </c>
+      <c r="D160">
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A161">
+        <v>12</v>
+      </c>
+      <c r="B161" t="s">
+        <v>179</v>
+      </c>
+      <c r="C161">
+        <v>46.5</v>
+      </c>
+      <c r="D161">
+        <v>-4.5</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A162">
+        <v>12</v>
+      </c>
+      <c r="B162" t="s">
+        <v>180</v>
+      </c>
+      <c r="C162">
+        <v>47.5</v>
+      </c>
+      <c r="D162">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A163">
+        <v>12</v>
+      </c>
+      <c r="B163" t="s">
+        <v>181</v>
+      </c>
+      <c r="C163">
+        <v>46.5</v>
+      </c>
+      <c r="D163">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
run initial lines for week 13
</commit_message>
<xml_diff>
--- a/betting_lines_open_2025.xlsx
+++ b/betting_lines_open_2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\Football-DNA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E769E31F-6F2E-44B4-9428-CD67B7365576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CBAD9B-26D8-4443-A15A-D46E41DB00A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="1" xr2:uid="{38E66C5D-58C4-4402-8F4D-2FF7B602BD04}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="11370" firstSheet="1" activeTab="1" xr2:uid="{38E66C5D-58C4-4402-8F4D-2FF7B602BD04}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 11" sheetId="9" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="198">
   <si>
     <t>game</t>
   </si>
@@ -583,6 +583,54 @@
   </si>
   <si>
     <t>CAR_SF</t>
+  </si>
+  <si>
+    <t>GB_DET</t>
+  </si>
+  <si>
+    <t>KC_DAL</t>
+  </si>
+  <si>
+    <t>CIN_BAL</t>
+  </si>
+  <si>
+    <t>CHI_PHI</t>
+  </si>
+  <si>
+    <t>HOU_IND</t>
+  </si>
+  <si>
+    <t>SF_CLE</t>
+  </si>
+  <si>
+    <t>ARI_TB</t>
+  </si>
+  <si>
+    <t>NO_MIA</t>
+  </si>
+  <si>
+    <t>LA_CAR</t>
+  </si>
+  <si>
+    <t>ATL_NYJ</t>
+  </si>
+  <si>
+    <t>JAX_TEN</t>
+  </si>
+  <si>
+    <t>MIN_SEA</t>
+  </si>
+  <si>
+    <t>LV_LAC</t>
+  </si>
+  <si>
+    <t>BUF_PIT</t>
+  </si>
+  <si>
+    <t>DEN_WAS</t>
+  </si>
+  <si>
+    <t>NYG_NE</t>
   </si>
 </sst>
 </file>
@@ -1145,10 +1193,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FD36202-D83D-42C3-9E22-D680F63FC59E}">
-  <dimension ref="A1:D163"/>
+  <dimension ref="A1:D179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="C149" sqref="C149"/>
+    <sheetView tabSelected="1" topLeftCell="A158" workbookViewId="0">
+      <selection activeCell="E165" sqref="E165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3435,6 +3483,230 @@
         <v>7</v>
       </c>
     </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A164">
+        <v>13</v>
+      </c>
+      <c r="B164" t="s">
+        <v>182</v>
+      </c>
+      <c r="C164">
+        <v>48.5</v>
+      </c>
+      <c r="D164">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A165">
+        <v>13</v>
+      </c>
+      <c r="B165" t="s">
+        <v>183</v>
+      </c>
+      <c r="C165">
+        <v>47.5</v>
+      </c>
+      <c r="D165">
+        <v>-5.5</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A166">
+        <v>13</v>
+      </c>
+      <c r="B166" t="s">
+        <v>184</v>
+      </c>
+      <c r="C166">
+        <v>49.5</v>
+      </c>
+      <c r="D166">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A167">
+        <v>13</v>
+      </c>
+      <c r="B167" t="s">
+        <v>185</v>
+      </c>
+      <c r="C167">
+        <v>46.5</v>
+      </c>
+      <c r="D167">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A168">
+        <v>13</v>
+      </c>
+      <c r="B168" t="s">
+        <v>186</v>
+      </c>
+      <c r="C168">
+        <v>44.5</v>
+      </c>
+      <c r="D168">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A169">
+        <v>13</v>
+      </c>
+      <c r="B169" t="s">
+        <v>187</v>
+      </c>
+      <c r="C169">
+        <v>42.5</v>
+      </c>
+      <c r="D169">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A170">
+        <v>13</v>
+      </c>
+      <c r="B170" t="s">
+        <v>188</v>
+      </c>
+      <c r="C170">
+        <v>48.5</v>
+      </c>
+      <c r="D170">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A171">
+        <v>13</v>
+      </c>
+      <c r="B171" t="s">
+        <v>189</v>
+      </c>
+      <c r="C171">
+        <v>44.5</v>
+      </c>
+      <c r="D171">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A172">
+        <v>13</v>
+      </c>
+      <c r="B172" t="s">
+        <v>190</v>
+      </c>
+      <c r="C172">
+        <v>45.5</v>
+      </c>
+      <c r="D172">
+        <v>-3.5</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A173">
+        <v>13</v>
+      </c>
+      <c r="B173" t="s">
+        <v>191</v>
+      </c>
+      <c r="C173">
+        <v>43.5</v>
+      </c>
+      <c r="D173">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A174">
+        <v>13</v>
+      </c>
+      <c r="B174" t="s">
+        <v>192</v>
+      </c>
+      <c r="C174">
+        <v>45.5</v>
+      </c>
+      <c r="D174">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A175">
+        <v>13</v>
+      </c>
+      <c r="B175" t="s">
+        <v>193</v>
+      </c>
+      <c r="C175">
+        <v>43.5</v>
+      </c>
+      <c r="D175">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A176">
+        <v>13</v>
+      </c>
+      <c r="B176" t="s">
+        <v>194</v>
+      </c>
+      <c r="C176">
+        <v>44.5</v>
+      </c>
+      <c r="D176">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A177">
+        <v>13</v>
+      </c>
+      <c r="B177" t="s">
+        <v>195</v>
+      </c>
+      <c r="C177">
+        <v>46.5</v>
+      </c>
+      <c r="D177">
+        <v>-4.5</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A178">
+        <v>13</v>
+      </c>
+      <c r="B178" t="s">
+        <v>196</v>
+      </c>
+      <c r="C178">
+        <v>46.5</v>
+      </c>
+      <c r="D178">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A179">
+        <v>13</v>
+      </c>
+      <c r="B179" t="s">
+        <v>197</v>
+      </c>
+      <c r="C179">
+        <v>42.5</v>
+      </c>
+      <c r="D179">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
initial run week 14
</commit_message>
<xml_diff>
--- a/betting_lines_open_2025.xlsx
+++ b/betting_lines_open_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\Football-DNA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CBAD9B-26D8-4443-A15A-D46E41DB00A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7BB4E8-5751-41C2-ABA4-C0FA20D22A4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="11370" firstSheet="1" activeTab="1" xr2:uid="{38E66C5D-58C4-4402-8F4D-2FF7B602BD04}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="212">
   <si>
     <t>game</t>
   </si>
@@ -631,6 +631,48 @@
   </si>
   <si>
     <t>NYG_NE</t>
+  </si>
+  <si>
+    <t>DAL_DET</t>
+  </si>
+  <si>
+    <t>WAS_MIN</t>
+  </si>
+  <si>
+    <t>MIA_NYJ</t>
+  </si>
+  <si>
+    <t>TEN_CLE</t>
+  </si>
+  <si>
+    <t>PIT_BAL</t>
+  </si>
+  <si>
+    <t>SEA_ATL</t>
+  </si>
+  <si>
+    <t>IND_JAX</t>
+  </si>
+  <si>
+    <t>NO_TB</t>
+  </si>
+  <si>
+    <t>CIN_BUF</t>
+  </si>
+  <si>
+    <t>DEN_LV</t>
+  </si>
+  <si>
+    <t>CHI_GB</t>
+  </si>
+  <si>
+    <t>LA_ARI</t>
+  </si>
+  <si>
+    <t>HOU_KC</t>
+  </si>
+  <si>
+    <t>PHI_LAC</t>
   </si>
 </sst>
 </file>
@@ -1193,10 +1235,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FD36202-D83D-42C3-9E22-D680F63FC59E}">
-  <dimension ref="A1:D179"/>
+  <dimension ref="A1:D193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A158" workbookViewId="0">
-      <selection activeCell="E165" sqref="E165"/>
+    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="E179" sqref="E179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3707,6 +3749,202 @@
         <v>3</v>
       </c>
     </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A180">
+        <v>14</v>
+      </c>
+      <c r="B180" t="s">
+        <v>198</v>
+      </c>
+      <c r="C180">
+        <v>48.5</v>
+      </c>
+      <c r="D180">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A181">
+        <v>14</v>
+      </c>
+      <c r="B181" t="s">
+        <v>199</v>
+      </c>
+      <c r="C181">
+        <v>47.5</v>
+      </c>
+      <c r="D181">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A182">
+        <v>14</v>
+      </c>
+      <c r="B182" t="s">
+        <v>200</v>
+      </c>
+      <c r="C182">
+        <v>43.5</v>
+      </c>
+      <c r="D182">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A183">
+        <v>14</v>
+      </c>
+      <c r="B183" t="s">
+        <v>201</v>
+      </c>
+      <c r="C183">
+        <v>41.5</v>
+      </c>
+      <c r="D183">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A184">
+        <v>14</v>
+      </c>
+      <c r="B184" t="s">
+        <v>202</v>
+      </c>
+      <c r="C184">
+        <v>46.5</v>
+      </c>
+      <c r="D184">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A185">
+        <v>14</v>
+      </c>
+      <c r="B185" t="s">
+        <v>203</v>
+      </c>
+      <c r="C185">
+        <v>45.5</v>
+      </c>
+      <c r="D185">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A186">
+        <v>14</v>
+      </c>
+      <c r="B186" t="s">
+        <v>204</v>
+      </c>
+      <c r="C186">
+        <v>46.5</v>
+      </c>
+      <c r="D186">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A187">
+        <v>14</v>
+      </c>
+      <c r="B187" t="s">
+        <v>205</v>
+      </c>
+      <c r="C187">
+        <v>45.5</v>
+      </c>
+      <c r="D187">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A188">
+        <v>14</v>
+      </c>
+      <c r="B188" t="s">
+        <v>206</v>
+      </c>
+      <c r="C188">
+        <v>49.5</v>
+      </c>
+      <c r="D188">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A189">
+        <v>14</v>
+      </c>
+      <c r="B189" t="s">
+        <v>207</v>
+      </c>
+      <c r="C189">
+        <v>43.5</v>
+      </c>
+      <c r="D189">
+        <v>-3.5</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A190">
+        <v>14</v>
+      </c>
+      <c r="B190" t="s">
+        <v>208</v>
+      </c>
+      <c r="C190">
+        <v>46.5</v>
+      </c>
+      <c r="D190">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A191">
+        <v>14</v>
+      </c>
+      <c r="B191" t="s">
+        <v>209</v>
+      </c>
+      <c r="C191">
+        <v>47.5</v>
+      </c>
+      <c r="D191">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A192">
+        <v>14</v>
+      </c>
+      <c r="B192" t="s">
+        <v>210</v>
+      </c>
+      <c r="C192">
+        <v>45.5</v>
+      </c>
+      <c r="D192">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A193">
+        <v>14</v>
+      </c>
+      <c r="B193" t="s">
+        <v>211</v>
+      </c>
+      <c r="C193">
+        <v>45.5</v>
+      </c>
+      <c r="D193">
+        <v>-2.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update data to use weighted rolling averages + initial week 15 run
</commit_message>
<xml_diff>
--- a/betting_lines_open_2025.xlsx
+++ b/betting_lines_open_2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\Football-DNA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7BB4E8-5751-41C2-ABA4-C0FA20D22A4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0703718D-2505-452C-A4DA-59EDA99EEC89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="11370" firstSheet="1" activeTab="1" xr2:uid="{38E66C5D-58C4-4402-8F4D-2FF7B602BD04}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="1" xr2:uid="{38E66C5D-58C4-4402-8F4D-2FF7B602BD04}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 11" sheetId="9" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="228">
   <si>
     <t>game</t>
   </si>
@@ -673,6 +673,54 @@
   </si>
   <si>
     <t>PHI_LAC</t>
+  </si>
+  <si>
+    <t>ATL_TB</t>
+  </si>
+  <si>
+    <t>LAC_KC</t>
+  </si>
+  <si>
+    <t>NYJ_JAX</t>
+  </si>
+  <si>
+    <t>BUF_NE</t>
+  </si>
+  <si>
+    <t>ARI_HOU</t>
+  </si>
+  <si>
+    <t>BAL_CIN</t>
+  </si>
+  <si>
+    <t>CLE_CHI</t>
+  </si>
+  <si>
+    <t>LV_PHI</t>
+  </si>
+  <si>
+    <t>WAS_NYG</t>
+  </si>
+  <si>
+    <t>DET_LA</t>
+  </si>
+  <si>
+    <t>CAR_NO</t>
+  </si>
+  <si>
+    <t>GB_DEN</t>
+  </si>
+  <si>
+    <t>TEN_SF</t>
+  </si>
+  <si>
+    <t>IND_SEA</t>
+  </si>
+  <si>
+    <t>MIN_DAL</t>
+  </si>
+  <si>
+    <t>MIA_PIT</t>
   </si>
 </sst>
 </file>
@@ -1235,10 +1283,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FD36202-D83D-42C3-9E22-D680F63FC59E}">
-  <dimension ref="A1:D193"/>
+  <dimension ref="A1:D209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
-      <selection activeCell="E179" sqref="E179"/>
+    <sheetView tabSelected="1" topLeftCell="A188" workbookViewId="0">
+      <selection activeCell="D194" sqref="D194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3945,6 +3993,230 @@
         <v>-2.5</v>
       </c>
     </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A194">
+        <v>15</v>
+      </c>
+      <c r="B194" t="s">
+        <v>212</v>
+      </c>
+      <c r="C194">
+        <v>47.5</v>
+      </c>
+      <c r="D194">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A195">
+        <v>15</v>
+      </c>
+      <c r="B195" t="s">
+        <v>213</v>
+      </c>
+      <c r="C195">
+        <v>45.5</v>
+      </c>
+      <c r="D195">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A196">
+        <v>15</v>
+      </c>
+      <c r="B196" t="s">
+        <v>214</v>
+      </c>
+      <c r="C196">
+        <v>43.5</v>
+      </c>
+      <c r="D196">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A197">
+        <v>15</v>
+      </c>
+      <c r="B197" t="s">
+        <v>215</v>
+      </c>
+      <c r="C197">
+        <v>46.5</v>
+      </c>
+      <c r="D197">
+        <v>-4.5</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A198">
+        <v>15</v>
+      </c>
+      <c r="B198" t="s">
+        <v>216</v>
+      </c>
+      <c r="C198">
+        <v>45.5</v>
+      </c>
+      <c r="D198">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A199">
+        <v>15</v>
+      </c>
+      <c r="B199" t="s">
+        <v>217</v>
+      </c>
+      <c r="C199">
+        <v>49.5</v>
+      </c>
+      <c r="D199">
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A200">
+        <v>15</v>
+      </c>
+      <c r="B200" t="s">
+        <v>218</v>
+      </c>
+      <c r="C200">
+        <v>42.5</v>
+      </c>
+      <c r="D200">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A201">
+        <v>15</v>
+      </c>
+      <c r="B201" t="s">
+        <v>219</v>
+      </c>
+      <c r="C201">
+        <v>44.5</v>
+      </c>
+      <c r="D201">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A202">
+        <v>15</v>
+      </c>
+      <c r="B202" t="s">
+        <v>220</v>
+      </c>
+      <c r="C202">
+        <v>45.5</v>
+      </c>
+      <c r="D202">
+        <v>-4.5</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A203">
+        <v>15</v>
+      </c>
+      <c r="B203" t="s">
+        <v>221</v>
+      </c>
+      <c r="C203">
+        <v>48.5</v>
+      </c>
+      <c r="D203">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A204">
+        <v>15</v>
+      </c>
+      <c r="B204" t="s">
+        <v>222</v>
+      </c>
+      <c r="C204">
+        <v>43.5</v>
+      </c>
+      <c r="D204">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A205">
+        <v>15</v>
+      </c>
+      <c r="B205" t="s">
+        <v>223</v>
+      </c>
+      <c r="C205">
+        <v>44.5</v>
+      </c>
+      <c r="D205">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A206">
+        <v>15</v>
+      </c>
+      <c r="B206" t="s">
+        <v>224</v>
+      </c>
+      <c r="C206">
+        <v>45.5</v>
+      </c>
+      <c r="D206">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A207">
+        <v>15</v>
+      </c>
+      <c r="B207" t="s">
+        <v>225</v>
+      </c>
+      <c r="C207">
+        <v>44.5</v>
+      </c>
+      <c r="D207">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A208">
+        <v>15</v>
+      </c>
+      <c r="B208" t="s">
+        <v>226</v>
+      </c>
+      <c r="C208">
+        <v>45.5</v>
+      </c>
+      <c r="D208">
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A209">
+        <v>15</v>
+      </c>
+      <c r="B209" t="s">
+        <v>227</v>
+      </c>
+      <c r="C209">
+        <v>44.5</v>
+      </c>
+      <c r="D209">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
initial week 16 run
</commit_message>
<xml_diff>
--- a/betting_lines_open_2025.xlsx
+++ b/betting_lines_open_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\Football-DNA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5103F9-6D6A-42D4-9494-8372CAE4AD8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC119F7-1DA2-41E5-95B3-3054530DA090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="1" xr2:uid="{38E66C5D-58C4-4402-8F4D-2FF7B602BD04}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="245">
   <si>
     <t>game</t>
   </si>
@@ -724,6 +724,54 @@
   </si>
   <si>
     <t>PIT_CIN</t>
+  </si>
+  <si>
+    <t>LA_SEA</t>
+  </si>
+  <si>
+    <t>PHI_WAS</t>
+  </si>
+  <si>
+    <t>GB_CHI</t>
+  </si>
+  <si>
+    <t>BUF_CLE</t>
+  </si>
+  <si>
+    <t>NYJ_NO</t>
+  </si>
+  <si>
+    <t>MIN_NYG</t>
+  </si>
+  <si>
+    <t>TB_CAR</t>
+  </si>
+  <si>
+    <t>KC_TEN</t>
+  </si>
+  <si>
+    <t>LAC_DAL</t>
+  </si>
+  <si>
+    <t>CIN_MIA</t>
+  </si>
+  <si>
+    <t>ATL_ARI</t>
+  </si>
+  <si>
+    <t>JAX_DEN</t>
+  </si>
+  <si>
+    <t>PIT_DET</t>
+  </si>
+  <si>
+    <t>LV_HOU</t>
+  </si>
+  <si>
+    <t>NE_BAL</t>
+  </si>
+  <si>
+    <t>SF_IND</t>
   </si>
 </sst>
 </file>
@@ -1286,10 +1334,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FD36202-D83D-42C3-9E22-D680F63FC59E}">
-  <dimension ref="A1:D209"/>
+  <dimension ref="A1:D225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
+      <selection activeCell="D210" sqref="D210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4220,6 +4268,230 @@
         <v>3</v>
       </c>
     </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A210">
+        <v>16</v>
+      </c>
+      <c r="B210" t="s">
+        <v>229</v>
+      </c>
+      <c r="C210">
+        <v>44.5</v>
+      </c>
+      <c r="D210">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A211">
+        <v>16</v>
+      </c>
+      <c r="B211" t="s">
+        <v>230</v>
+      </c>
+      <c r="C211">
+        <v>48.5</v>
+      </c>
+      <c r="D211">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A212">
+        <v>16</v>
+      </c>
+      <c r="B212" t="s">
+        <v>231</v>
+      </c>
+      <c r="C212">
+        <v>45.5</v>
+      </c>
+      <c r="D212">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A213">
+        <v>16</v>
+      </c>
+      <c r="B213" t="s">
+        <v>232</v>
+      </c>
+      <c r="C213">
+        <v>43.5</v>
+      </c>
+      <c r="D213">
+        <v>-8.5</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A214">
+        <v>16</v>
+      </c>
+      <c r="B214" t="s">
+        <v>233</v>
+      </c>
+      <c r="C214">
+        <v>41.5</v>
+      </c>
+      <c r="D214">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A215">
+        <v>16</v>
+      </c>
+      <c r="B215" t="s">
+        <v>234</v>
+      </c>
+      <c r="C215">
+        <v>42.5</v>
+      </c>
+      <c r="D215">
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A216">
+        <v>16</v>
+      </c>
+      <c r="B216" t="s">
+        <v>235</v>
+      </c>
+      <c r="C216">
+        <v>47.5</v>
+      </c>
+      <c r="D216">
+        <v>-3.5</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A217">
+        <v>16</v>
+      </c>
+      <c r="B217" t="s">
+        <v>236</v>
+      </c>
+      <c r="C217">
+        <v>44.5</v>
+      </c>
+      <c r="D217">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A218">
+        <v>16</v>
+      </c>
+      <c r="B218" t="s">
+        <v>237</v>
+      </c>
+      <c r="C218">
+        <v>46.5</v>
+      </c>
+      <c r="D218">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A219">
+        <v>16</v>
+      </c>
+      <c r="B219" t="s">
+        <v>238</v>
+      </c>
+      <c r="C219">
+        <v>48.5</v>
+      </c>
+      <c r="D219">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A220">
+        <v>16</v>
+      </c>
+      <c r="B220" t="s">
+        <v>239</v>
+      </c>
+      <c r="C220">
+        <v>46.5</v>
+      </c>
+      <c r="D220">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A221">
+        <v>16</v>
+      </c>
+      <c r="B221" t="s">
+        <v>240</v>
+      </c>
+      <c r="C221">
+        <v>45.5</v>
+      </c>
+      <c r="D221">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A222">
+        <v>16</v>
+      </c>
+      <c r="B222" t="s">
+        <v>241</v>
+      </c>
+      <c r="C222">
+        <v>45.5</v>
+      </c>
+      <c r="D222">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A223">
+        <v>16</v>
+      </c>
+      <c r="B223" t="s">
+        <v>242</v>
+      </c>
+      <c r="C223">
+        <v>43.5</v>
+      </c>
+      <c r="D223">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A224">
+        <v>16</v>
+      </c>
+      <c r="B224" t="s">
+        <v>243</v>
+      </c>
+      <c r="C224">
+        <v>46.5</v>
+      </c>
+      <c r="D224">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A225">
+        <v>16</v>
+      </c>
+      <c r="B225" t="s">
+        <v>244</v>
+      </c>
+      <c r="C225">
+        <v>46.5</v>
+      </c>
+      <c r="D225">
+        <v>-3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
initial week 1 run
</commit_message>
<xml_diff>
--- a/betting_lines_open_2025.xlsx
+++ b/betting_lines_open_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\Football-DNA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC119F7-1DA2-41E5-95B3-3054530DA090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E897BC7-8ABB-46FE-A1A6-8BB22DE89557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="1" xr2:uid="{38E66C5D-58C4-4402-8F4D-2FF7B602BD04}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="261">
   <si>
     <t>game</t>
   </si>
@@ -772,6 +772,54 @@
   </si>
   <si>
     <t>SF_IND</t>
+  </si>
+  <si>
+    <t>DAL_WAS</t>
+  </si>
+  <si>
+    <t>DET_MIN</t>
+  </si>
+  <si>
+    <t>DEN_KC</t>
+  </si>
+  <si>
+    <t>HOU_LAC</t>
+  </si>
+  <si>
+    <t>BAL_GB</t>
+  </si>
+  <si>
+    <t>ARI_CIN</t>
+  </si>
+  <si>
+    <t>SEA_CAR</t>
+  </si>
+  <si>
+    <t>PIT_CLE</t>
+  </si>
+  <si>
+    <t>NO_TEN</t>
+  </si>
+  <si>
+    <t>TB_MIA</t>
+  </si>
+  <si>
+    <t>JAX_IND</t>
+  </si>
+  <si>
+    <t>NE_NYJ</t>
+  </si>
+  <si>
+    <t>NYG_LV</t>
+  </si>
+  <si>
+    <t>PHI_BUF</t>
+  </si>
+  <si>
+    <t>CHI_SF</t>
+  </si>
+  <si>
+    <t>LA_ATL</t>
   </si>
 </sst>
 </file>
@@ -1334,10 +1382,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FD36202-D83D-42C3-9E22-D680F63FC59E}">
-  <dimension ref="A1:D225"/>
+  <dimension ref="A1:D241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
-      <selection activeCell="D210" sqref="D210"/>
+    <sheetView tabSelected="1" topLeftCell="A220" workbookViewId="0">
+      <selection activeCell="I229" sqref="I229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4492,6 +4540,230 @@
         <v>-3</v>
       </c>
     </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A226">
+        <v>17</v>
+      </c>
+      <c r="B226" t="s">
+        <v>245</v>
+      </c>
+      <c r="C226">
+        <v>47.5</v>
+      </c>
+      <c r="D226">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A227">
+        <v>17</v>
+      </c>
+      <c r="B227" t="s">
+        <v>246</v>
+      </c>
+      <c r="C227">
+        <v>46.5</v>
+      </c>
+      <c r="D227">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A228">
+        <v>17</v>
+      </c>
+      <c r="B228" t="s">
+        <v>247</v>
+      </c>
+      <c r="C228">
+        <v>44.5</v>
+      </c>
+      <c r="D228">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A229">
+        <v>17</v>
+      </c>
+      <c r="B229" t="s">
+        <v>248</v>
+      </c>
+      <c r="C229">
+        <v>43.5</v>
+      </c>
+      <c r="D229">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A230">
+        <v>17</v>
+      </c>
+      <c r="B230" t="s">
+        <v>249</v>
+      </c>
+      <c r="C230">
+        <v>46.5</v>
+      </c>
+      <c r="D230">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A231">
+        <v>17</v>
+      </c>
+      <c r="B231" t="s">
+        <v>250</v>
+      </c>
+      <c r="C231">
+        <v>47.5</v>
+      </c>
+      <c r="D231">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A232">
+        <v>17</v>
+      </c>
+      <c r="B232" t="s">
+        <v>251</v>
+      </c>
+      <c r="C232">
+        <v>43.5</v>
+      </c>
+      <c r="D232">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A233">
+        <v>17</v>
+      </c>
+      <c r="B233" t="s">
+        <v>252</v>
+      </c>
+      <c r="C233">
+        <v>40.5</v>
+      </c>
+      <c r="D233">
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A234">
+        <v>17</v>
+      </c>
+      <c r="B234" t="s">
+        <v>253</v>
+      </c>
+      <c r="C234">
+        <v>42.5</v>
+      </c>
+      <c r="D234">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A235">
+        <v>17</v>
+      </c>
+      <c r="B235" t="s">
+        <v>254</v>
+      </c>
+      <c r="C235">
+        <v>47.5</v>
+      </c>
+      <c r="D235">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A236">
+        <v>17</v>
+      </c>
+      <c r="B236" t="s">
+        <v>255</v>
+      </c>
+      <c r="C236">
+        <v>45.5</v>
+      </c>
+      <c r="D236">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A237">
+        <v>17</v>
+      </c>
+      <c r="B237" t="s">
+        <v>256</v>
+      </c>
+      <c r="C237">
+        <v>41.5</v>
+      </c>
+      <c r="D237">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A238">
+        <v>17</v>
+      </c>
+      <c r="B238" t="s">
+        <v>257</v>
+      </c>
+      <c r="C238">
+        <v>42.5</v>
+      </c>
+      <c r="D238">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A239">
+        <v>17</v>
+      </c>
+      <c r="B239" t="s">
+        <v>258</v>
+      </c>
+      <c r="C239">
+        <v>46.5</v>
+      </c>
+      <c r="D239">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A240">
+        <v>17</v>
+      </c>
+      <c r="B240" t="s">
+        <v>259</v>
+      </c>
+      <c r="C240">
+        <v>46.5</v>
+      </c>
+      <c r="D240">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A241">
+        <v>17</v>
+      </c>
+      <c r="B241" t="s">
+        <v>260</v>
+      </c>
+      <c r="C241">
+        <v>46.5</v>
+      </c>
+      <c r="D241">
+        <v>-3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
initial run WC playoffs
</commit_message>
<xml_diff>
--- a/betting_lines_open_2025.xlsx
+++ b/betting_lines_open_2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\Football-DNA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7281098-47C2-494C-9DCA-D65E8E467FA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C55071-7697-4F6D-9FDF-B993039B7D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="11370" firstSheet="1" activeTab="1" xr2:uid="{38E66C5D-58C4-4402-8F4D-2FF7B602BD04}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="1" xr2:uid="{38E66C5D-58C4-4402-8F4D-2FF7B602BD04}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 11" sheetId="9" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="281">
   <si>
     <t>game</t>
   </si>
@@ -868,6 +868,18 @@
   </si>
   <si>
     <t>TEN_JAX</t>
+  </si>
+  <si>
+    <t>BUF_JAX</t>
+  </si>
+  <si>
+    <t>SF_PHI</t>
+  </si>
+  <si>
+    <t>LAC_NE</t>
+  </si>
+  <si>
+    <t>HOU_PIT</t>
   </si>
 </sst>
 </file>
@@ -1430,10 +1442,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FD36202-D83D-42C3-9E22-D680F63FC59E}">
-  <dimension ref="A1:D257"/>
+  <dimension ref="A1:D263"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A236" workbookViewId="0">
-      <selection activeCell="E241" sqref="E241"/>
+    <sheetView tabSelected="1" topLeftCell="A247" workbookViewId="0">
+      <selection activeCell="D264" sqref="D264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5036,6 +5048,90 @@
         <v>4.5</v>
       </c>
     </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A258">
+        <v>19</v>
+      </c>
+      <c r="B258" t="s">
+        <v>190</v>
+      </c>
+      <c r="C258">
+        <v>46.5</v>
+      </c>
+      <c r="D258">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A259">
+        <v>19</v>
+      </c>
+      <c r="B259" t="s">
+        <v>231</v>
+      </c>
+      <c r="C259">
+        <v>45.5</v>
+      </c>
+      <c r="D259">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A260">
+        <v>19</v>
+      </c>
+      <c r="B260" t="s">
+        <v>277</v>
+      </c>
+      <c r="C260">
+        <v>51.5</v>
+      </c>
+      <c r="D260">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A261">
+        <v>19</v>
+      </c>
+      <c r="B261" t="s">
+        <v>278</v>
+      </c>
+      <c r="C261">
+        <v>46.5</v>
+      </c>
+      <c r="D261">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A262">
+        <v>19</v>
+      </c>
+      <c r="B262" t="s">
+        <v>279</v>
+      </c>
+      <c r="C262">
+        <v>45.5</v>
+      </c>
+      <c r="D262">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A263">
+        <v>19</v>
+      </c>
+      <c r="B263" t="s">
+        <v>280</v>
+      </c>
+      <c r="C263">
+        <v>38.5</v>
+      </c>
+      <c r="D263">
+        <v>-3.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
initial divisional round run
</commit_message>
<xml_diff>
--- a/betting_lines_open_2025.xlsx
+++ b/betting_lines_open_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\Football-DNA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C55071-7697-4F6D-9FDF-B993039B7D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478BB39B-BE11-447B-AAB5-4984A4DCA61C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="1" xr2:uid="{38E66C5D-58C4-4402-8F4D-2FF7B602BD04}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="284">
   <si>
     <t>game</t>
   </si>
@@ -880,6 +880,15 @@
   </si>
   <si>
     <t>HOU_PIT</t>
+  </si>
+  <si>
+    <t>SF_SEA</t>
+  </si>
+  <si>
+    <t>LA_CHI</t>
+  </si>
+  <si>
+    <t>BUF_DEN</t>
   </si>
 </sst>
 </file>
@@ -1442,10 +1451,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FD36202-D83D-42C3-9E22-D680F63FC59E}">
-  <dimension ref="A1:D263"/>
+  <dimension ref="A1:D266"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A247" workbookViewId="0">
-      <selection activeCell="D264" sqref="D264"/>
+    <sheetView tabSelected="1" topLeftCell="A249" workbookViewId="0">
+      <selection activeCell="E264" sqref="E264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5132,6 +5141,48 @@
         <v>-3.5</v>
       </c>
     </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A264">
+        <v>20</v>
+      </c>
+      <c r="B264" t="s">
+        <v>281</v>
+      </c>
+      <c r="C264">
+        <v>46.5</v>
+      </c>
+      <c r="D264">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A265">
+        <v>20</v>
+      </c>
+      <c r="B265" t="s">
+        <v>282</v>
+      </c>
+      <c r="C265">
+        <v>51.5</v>
+      </c>
+      <c r="D265">
+        <v>-4.5</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A266">
+        <v>20</v>
+      </c>
+      <c r="B266" t="s">
+        <v>283</v>
+      </c>
+      <c r="C266">
+        <v>46.5</v>
+      </c>
+      <c r="D266">
+        <v>-1.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated opening lines spreadsheet
</commit_message>
<xml_diff>
--- a/betting_lines_open_2025.xlsx
+++ b/betting_lines_open_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\Football-DNA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478BB39B-BE11-447B-AAB5-4984A4DCA61C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A7DD824-5B27-41F2-BAF5-5D5A6B555E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="1" xr2:uid="{38E66C5D-58C4-4402-8F4D-2FF7B602BD04}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="285">
   <si>
     <t>game</t>
   </si>
@@ -889,6 +889,9 @@
   </si>
   <si>
     <t>BUF_DEN</t>
+  </si>
+  <si>
+    <t>HOU_NE</t>
   </si>
 </sst>
 </file>
@@ -1451,10 +1454,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FD36202-D83D-42C3-9E22-D680F63FC59E}">
-  <dimension ref="A1:D266"/>
+  <dimension ref="A1:D267"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A249" workbookViewId="0">
-      <selection activeCell="E264" sqref="E264"/>
+      <selection activeCell="D265" sqref="D265"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5152,7 +5155,7 @@
         <v>46.5</v>
       </c>
       <c r="D264">
-        <v>6.5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.35">
@@ -5181,6 +5184,20 @@
       </c>
       <c r="D266">
         <v>-1.5</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A267">
+        <v>20</v>
+      </c>
+      <c r="B267" t="s">
+        <v>284</v>
+      </c>
+      <c r="C267">
+        <v>43.5</v>
+      </c>
+      <c r="D267">
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
initial conf champ run
</commit_message>
<xml_diff>
--- a/betting_lines_open_2025.xlsx
+++ b/betting_lines_open_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\Football-DNA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A7DD824-5B27-41F2-BAF5-5D5A6B555E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A722B4-2B04-43BE-BC53-EEC1C4F2E71A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="1" xr2:uid="{38E66C5D-58C4-4402-8F4D-2FF7B602BD04}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="286">
   <si>
     <t>game</t>
   </si>
@@ -892,6 +892,9 @@
   </si>
   <si>
     <t>HOU_NE</t>
+  </si>
+  <si>
+    <t>NE_DEN</t>
   </si>
 </sst>
 </file>
@@ -1454,10 +1457,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FD36202-D83D-42C3-9E22-D680F63FC59E}">
-  <dimension ref="A1:D267"/>
+  <dimension ref="A1:D269"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A249" workbookViewId="0">
-      <selection activeCell="D265" sqref="D265"/>
+    <sheetView tabSelected="1" topLeftCell="A250" workbookViewId="0">
+      <selection activeCell="A268" sqref="A268:A269"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5200,6 +5203,34 @@
         <v>2.5</v>
       </c>
     </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A268">
+        <v>21</v>
+      </c>
+      <c r="B268" t="s">
+        <v>285</v>
+      </c>
+      <c r="C268">
+        <v>40.5</v>
+      </c>
+      <c r="D268">
+        <v>-5.5</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A269">
+        <v>21</v>
+      </c>
+      <c r="B269" t="s">
+        <v>229</v>
+      </c>
+      <c r="C269">
+        <v>47.5</v>
+      </c>
+      <c r="D269">
+        <v>1.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>